<commit_message>
updated excel and csv
updated names
</commit_message>
<xml_diff>
--- a/Excel data files/all teams logo.xlsx
+++ b/Excel data files/all teams logo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\powerbi_cricket_dash\Excel data files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFFA97D-57DB-4D65-AF7E-6ACA20362505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29616AAF-1A67-4038-8B14-262ED7CBB1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{FC8DCA95-93ED-484F-814E-78E565B9391F}"/>
+    <workbookView xWindow="1680" yWindow="2832" windowWidth="17280" windowHeight="8964" xr2:uid="{FC8DCA95-93ED-484F-814E-78E565B9391F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
   <si>
     <t>Logo</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t>Sunrisers Hyderabad Team</t>
+  </si>
+  <si>
+    <t>Rajasthan Royals T</t>
+  </si>
+  <si>
+    <t>Punjab Kings T</t>
   </si>
 </sst>
 </file>
@@ -625,7 +631,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,7 +766,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
         <v>54</v>
@@ -777,7 +783,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
         <v>53</v>

</xml_diff>